<commit_message>
Dagbækur fyrir alvöru karlmenn
</commit_message>
<xml_diff>
--- a/Dagbaekur/Vilhelm/Dagbok.xlsx
+++ b/Dagbaekur/Vilhelm/Dagbok.xlsx
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -807,18 +807,24 @@
       <c r="D27">
         <v>180</v>
       </c>
+      <c r="E27">
+        <v>180</v>
+      </c>
       <c r="J27">
         <f t="shared" ref="J27:J31" si="2">SUM(C27:I27)</f>
-        <v>180</v>
+        <v>360</v>
       </c>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" t="s">
         <v>2</v>
       </c>
+      <c r="E28">
+        <v>60</v>
+      </c>
       <c r="J28">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="2:10">
@@ -831,9 +837,12 @@
       <c r="D29">
         <v>120</v>
       </c>
+      <c r="E29">
+        <v>60</v>
+      </c>
       <c r="J29">
         <f t="shared" si="2"/>
-        <v>240</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="2:10">
@@ -867,7 +876,7 @@
       </c>
       <c r="J32">
         <f>SUM(J26:J31)</f>
-        <v>420</v>
+        <v>720</v>
       </c>
     </row>
     <row r="34" spans="2:10">
@@ -1128,7 +1137,7 @@
       </c>
       <c r="D57">
         <f t="shared" si="5"/>
-        <v>360</v>
+        <v>540</v>
       </c>
     </row>
     <row r="58" spans="2:10">
@@ -1137,7 +1146,7 @@
       </c>
       <c r="D58">
         <f t="shared" si="5"/>
-        <v>180</v>
+        <v>240</v>
       </c>
     </row>
     <row r="59" spans="2:10">
@@ -1146,7 +1155,7 @@
       </c>
       <c r="D59">
         <f t="shared" si="5"/>
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="60" spans="2:10">
@@ -1174,7 +1183,7 @@
       </c>
       <c r="D62" s="3">
         <f>SUM(D56:D61)</f>
-        <v>1020</v>
+        <v>1320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>